<commit_message>
experiment3 completed - dup
</commit_message>
<xml_diff>
--- a/experiments/experiment_3/notebooks/estrategias.xlsx
+++ b/experiments/experiment_3/notebooks/estrategias.xlsx
@@ -14,45 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
-  <si>
-    <t>Estratégia</t>
-  </si>
-  <si>
-    <t>Related</t>
-  </si>
-  <si>
-    <t>Visited</t>
-  </si>
-  <si>
-    <t>Final Selected</t>
-  </si>
-  <si>
-    <t>Precision</t>
-  </si>
-  <si>
-    <t>Recall</t>
-  </si>
-  <si>
-    <t>F-Measure</t>
-  </si>
-  <si>
-    <t>Final Precision</t>
-  </si>
-  <si>
-    <t>Final Recall</t>
-  </si>
-  <si>
-    <t>Final F-Measure</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>E1</t>
   </si>
   <si>
     <t>E2</t>
-  </si>
-  <si>
-    <t>E3</t>
   </si>
   <si>
     <t>E4</t>
@@ -422,53 +389,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:14">
+      <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="1">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="1">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="1">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="1">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="1">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="1">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="1">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="1">
         <v>9</v>
       </c>
+      <c r="L1" s="1">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
+    <row r="2" spans="1:14">
+      <c r="A2" s="1">
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>11</v>
@@ -480,232 +453,251 @@
         <v>11</v>
       </c>
       <c r="F2">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0.02282157676348548</v>
+      </c>
+      <c r="J2">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="K2">
+        <v>0.04435483870967741</v>
+      </c>
+      <c r="L2">
+        <v>0.02282157676348548</v>
+      </c>
+      <c r="M2">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="N2">
+        <v>0.04435483870967741</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="H2">
-        <v>0.04</v>
-      </c>
-      <c r="I2">
-        <v>0.02</v>
-      </c>
-      <c r="J2">
-        <v>0.79</v>
-      </c>
-      <c r="K2">
-        <v>0.04</v>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>933</v>
+      </c>
+      <c r="E3">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0.015005359056806</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0.02956705385427667</v>
+      </c>
+      <c r="L3">
+        <v>0.015005359056806</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>0.02956705385427667</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:14">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D4">
+        <v>502</v>
+      </c>
+      <c r="E4">
         <v>11</v>
       </c>
-      <c r="C3">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0.02191235059760956</v>
+      </c>
+      <c r="J4">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="K4">
+        <v>0.04263565891472869</v>
+      </c>
+      <c r="L4">
+        <v>0.02191235059760956</v>
+      </c>
+      <c r="M4">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="N4">
+        <v>0.04263565891472869</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>242</v>
+      </c>
+      <c r="E5">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0.0371900826446281</v>
+      </c>
+      <c r="J5">
+        <v>0.6428571428571429</v>
+      </c>
+      <c r="K5">
+        <v>0.0703125</v>
+      </c>
+      <c r="L5">
+        <v>0.0371900826446281</v>
+      </c>
+      <c r="M5">
+        <v>0.6428571428571429</v>
+      </c>
+      <c r="N5">
+        <v>0.0703125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
         <v>11</v>
       </c>
-      <c r="D3">
-        <v>548</v>
-      </c>
-      <c r="E3">
+      <c r="D6">
+        <v>424</v>
+      </c>
+      <c r="E6">
         <v>11</v>
       </c>
-      <c r="F3">
-        <v>0.02</v>
-      </c>
-      <c r="G3">
-        <v>0.79</v>
-      </c>
-      <c r="H3">
-        <v>0.04</v>
-      </c>
-      <c r="I3">
-        <v>0.02</v>
-      </c>
-      <c r="J3">
-        <v>0.79</v>
-      </c>
-      <c r="K3">
-        <v>0.04</v>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0.0259433962264151</v>
+      </c>
+      <c r="J6">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="K6">
+        <v>0.0502283105022831</v>
+      </c>
+      <c r="L6">
+        <v>0.0259433962264151</v>
+      </c>
+      <c r="M6">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="N6">
+        <v>0.0502283105022831</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>14</v>
-      </c>
-      <c r="D4">
-        <v>950</v>
-      </c>
-      <c r="E4">
-        <v>14</v>
-      </c>
-      <c r="F4">
-        <v>0.01</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>0.03</v>
-      </c>
-      <c r="I4">
-        <v>0.01</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>467</v>
-      </c>
-      <c r="E5">
-        <v>11</v>
-      </c>
-      <c r="F5">
-        <v>0.02</v>
-      </c>
-      <c r="G5">
-        <v>0.79</v>
-      </c>
-      <c r="H5">
-        <v>0.05</v>
-      </c>
-      <c r="I5">
-        <v>0.02</v>
-      </c>
-      <c r="J5">
-        <v>0.79</v>
-      </c>
-      <c r="K5">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>103</v>
-      </c>
-      <c r="E6">
-        <v>7</v>
-      </c>
-      <c r="F6">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="G6">
-        <v>0.5</v>
-      </c>
-      <c r="H6">
-        <v>0.12</v>
-      </c>
-      <c r="I6">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="J6">
-        <v>0.5</v>
-      </c>
-      <c r="K6">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
+    <row r="7" spans="1:14">
+      <c r="A7" s="1">
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7">
-        <v>331</v>
+        <v>275</v>
       </c>
       <c r="E7">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>0.79</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>0.03</v>
+        <v>0.03272727272727273</v>
       </c>
       <c r="J7">
-        <v>0.79</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="K7">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>180</v>
-      </c>
-      <c r="E8">
-        <v>8</v>
-      </c>
-      <c r="F8">
-        <v>0.04</v>
-      </c>
-      <c r="G8">
-        <v>0.57</v>
-      </c>
-      <c r="H8">
-        <v>0.08</v>
-      </c>
-      <c r="I8">
-        <v>0.04</v>
-      </c>
-      <c r="J8">
-        <v>0.57</v>
-      </c>
-      <c r="K8">
-        <v>0.08</v>
+        <v>0.06228373702422146</v>
+      </c>
+      <c r="L7">
+        <v>0.03272727272727273</v>
+      </c>
+      <c r="M7">
+        <v>0.6428571428571429</v>
+      </c>
+      <c r="N7">
+        <v>0.06228373702422146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajustes nos 3 notebooks
</commit_message>
<xml_diff>
--- a/experiments/experiment_3/notebooks/estrategias.xlsx
+++ b/experiments/experiment_3/notebooks/estrategias.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>E1</t>
   </si>
   <si>
     <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
   </si>
   <si>
     <t>E4</t>
@@ -389,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -447,7 +450,7 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="E2">
         <v>11</v>
@@ -462,22 +465,22 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0.02282157676348548</v>
+        <v>0.02291666666666667</v>
       </c>
       <c r="J2">
         <v>0.7857142857142857</v>
       </c>
       <c r="K2">
-        <v>0.04435483870967741</v>
+        <v>0.04453441295546558</v>
       </c>
       <c r="L2">
-        <v>0.02282157676348548</v>
+        <v>0.02291666666666667</v>
       </c>
       <c r="M2">
         <v>0.7857142857142857</v>
       </c>
       <c r="N2">
-        <v>0.04435483870967741</v>
+        <v>0.04453441295546558</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -491,7 +494,7 @@
         <v>14</v>
       </c>
       <c r="D3">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="E3">
         <v>14</v>
@@ -506,22 +509,22 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0.015005359056806</v>
+        <v>0.01502145922746781</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3">
-        <v>0.02956705385427667</v>
+        <v>0.02959830866807611</v>
       </c>
       <c r="L3">
-        <v>0.015005359056806</v>
+        <v>0.01502145922746781</v>
       </c>
       <c r="M3">
         <v>1</v>
       </c>
       <c r="N3">
-        <v>0.02956705385427667</v>
+        <v>0.02959830866807611</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -535,7 +538,7 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>502</v>
+        <v>442</v>
       </c>
       <c r="E4">
         <v>11</v>
@@ -550,22 +553,22 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0.02191235059760956</v>
+        <v>0.0248868778280543</v>
       </c>
       <c r="J4">
         <v>0.7857142857142857</v>
       </c>
       <c r="K4">
-        <v>0.04263565891472869</v>
+        <v>0.04824561403508772</v>
       </c>
       <c r="L4">
-        <v>0.02191235059760956</v>
+        <v>0.0248868778280543</v>
       </c>
       <c r="M4">
         <v>0.7857142857142857</v>
       </c>
       <c r="N4">
-        <v>0.04263565891472869</v>
+        <v>0.04824561403508772</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -576,13 +579,13 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D5">
-        <v>242</v>
+        <v>502</v>
       </c>
       <c r="E5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -594,22 +597,22 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0.0371900826446281</v>
+        <v>0.02191235059760956</v>
       </c>
       <c r="J5">
-        <v>0.6428571428571429</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="K5">
-        <v>0.0703125</v>
+        <v>0.04263565891472869</v>
       </c>
       <c r="L5">
-        <v>0.0371900826446281</v>
+        <v>0.02191235059760956</v>
       </c>
       <c r="M5">
-        <v>0.6428571428571429</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="N5">
-        <v>0.0703125</v>
+        <v>0.04263565891472869</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -620,13 +623,13 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6">
-        <v>424</v>
+        <v>242</v>
       </c>
       <c r="E6">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -638,22 +641,22 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0.0259433962264151</v>
+        <v>0.0371900826446281</v>
       </c>
       <c r="J6">
-        <v>0.7857142857142857</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="K6">
-        <v>0.0502283105022831</v>
+        <v>0.0703125</v>
       </c>
       <c r="L6">
-        <v>0.0259433962264151</v>
+        <v>0.0371900826446281</v>
       </c>
       <c r="M6">
-        <v>0.7857142857142857</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="N6">
-        <v>0.0502283105022831</v>
+        <v>0.0703125</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -664,39 +667,83 @@
         <v>5</v>
       </c>
       <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>424</v>
+      </c>
+      <c r="E7">
+        <v>11</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0.0259433962264151</v>
+      </c>
+      <c r="J7">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="K7">
+        <v>0.0502283105022831</v>
+      </c>
+      <c r="L7">
+        <v>0.0259433962264151</v>
+      </c>
+      <c r="M7">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="N7">
+        <v>0.0502283105022831</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
         <v>9</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>275</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>9</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
         <v>0.03272727272727273</v>
       </c>
-      <c r="J7">
+      <c r="J8">
         <v>0.6428571428571429</v>
       </c>
-      <c r="K7">
+      <c r="K8">
         <v>0.06228373702422146</v>
       </c>
-      <c r="L7">
+      <c r="L8">
         <v>0.03272727272727273</v>
       </c>
-      <c r="M7">
+      <c r="M8">
         <v>0.6428571428571429</v>
       </c>
-      <c r="N7">
+      <c r="N8">
         <v>0.06228373702422146</v>
       </c>
     </row>

</xml_diff>